<commit_message>
excel sheet & tesng xml file updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/OpenCart_TestData.xlsx
+++ b/src/test/resources/testdata/OpenCart_TestData.xlsx
@@ -96,28 +96,28 @@
     <t>878999999</t>
   </si>
   <si>
-    <t>ddhivya</t>
-  </si>
-  <si>
-    <t>aanjum</t>
-  </si>
-  <si>
-    <t>sshivender</t>
-  </si>
-  <si>
-    <t>nnaveen</t>
-  </si>
-  <si>
-    <t>dhivya11abc@gmail.com</t>
-  </si>
-  <si>
-    <t>anjum11abc@gmail.com</t>
-  </si>
-  <si>
-    <t>shiv11abc@gmail.com</t>
-  </si>
-  <si>
-    <t>naveen11abc@gmail.com</t>
+    <t>dddhivya</t>
+  </si>
+  <si>
+    <t>adanjum</t>
+  </si>
+  <si>
+    <t>sfshivender</t>
+  </si>
+  <si>
+    <t>nfnaveen</t>
+  </si>
+  <si>
+    <t>dhivya111abc@gmail.com</t>
+  </si>
+  <si>
+    <t>anjum111abc@gmail.com</t>
+  </si>
+  <si>
+    <t>shiv112abc@gmail.com</t>
+  </si>
+  <si>
+    <t>naveen11a2bc@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>